<commit_message>
analysis done on danish and bengali with correct parsing
</commit_message>
<xml_diff>
--- a/outputs/sem_score_sheets/sem_scores_analysis_zeroshot_da.xlsx
+++ b/outputs/sem_score_sheets/sem_scores_analysis_zeroshot_da.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4539973435474426</v>
+        <v>0.4556138485070078</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02563050126273778</v>
+        <v>0.02585973950267152</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.3747600586542418</v>
+        <v>0.3732759649991058</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03298650043576561</v>
+        <v>0.03282961426643728</v>
       </c>
     </row>
     <row r="4">
@@ -494,10 +494,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.324294145100496</v>
+        <v>0.3266774160878911</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02467573350408211</v>
+        <v>0.02492181048694208</v>
       </c>
     </row>
     <row r="5">
@@ -512,10 +512,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1937774555181222</v>
+        <v>0.195774715798907</v>
       </c>
       <c r="D5" t="n">
-        <v>0.003415445446509846</v>
+        <v>0.003796050459893252</v>
       </c>
     </row>
     <row r="6">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3871543732741321</v>
+        <v>0.3906183618996238</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02269727087549189</v>
+        <v>0.02355869632477699</v>
       </c>
     </row>
     <row r="7">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3922947794907277</v>
+        <v>0.3985555628723957</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02754605045318954</v>
+        <v>0.03025583084042707</v>
       </c>
     </row>
     <row r="8">
@@ -566,10 +566,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3237662471854275</v>
+        <v>0.3331450224627091</v>
       </c>
       <c r="D8" t="n">
-        <v>0.02301367938048235</v>
+        <v>0.02445492832969585</v>
       </c>
     </row>
     <row r="9">
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4068448461326523</v>
+        <v>0.4063456806459282</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02695653787658921</v>
+        <v>0.02663870627794609</v>
       </c>
     </row>
     <row r="10">
@@ -602,10 +602,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.4233326197788119</v>
+        <v>0.4225102493798007</v>
       </c>
       <c r="D10" t="n">
-        <v>0.03281527496280936</v>
+        <v>0.03278623945329751</v>
       </c>
     </row>
     <row r="11">
@@ -620,10 +620,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3990445340564166</v>
+        <v>0.4055499661512212</v>
       </c>
       <c r="D11" t="n">
-        <v>0.03293240728846523</v>
+        <v>0.03404502253521277</v>
       </c>
     </row>
     <row r="12">
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3748530882529597</v>
+        <v>0.3732804392610282</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03463412239933993</v>
+        <v>0.03456729437841123</v>
       </c>
     </row>
     <row r="13">
@@ -656,10 +656,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.3235834821131865</v>
+        <v>0.3272709149099954</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0237457787763674</v>
+        <v>0.02405916697052345</v>
       </c>
     </row>
     <row r="14">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.3861707945503193</v>
+        <v>0.3872297676156624</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02994872160144692</v>
+        <v>0.02973057817280951</v>
       </c>
     </row>
     <row r="15">
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.3592439875176843</v>
+        <v>0.3596599845188618</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03268539615644801</v>
+        <v>0.03266446457420254</v>
       </c>
     </row>
     <row r="16">
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.3575009512897943</v>
+        <v>0.3592414334528549</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02404071720810639</v>
+        <v>0.02409583787381832</v>
       </c>
     </row>
     <row r="17">
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3422769261677246</v>
+        <v>0.3436107846250926</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02466210471142661</v>
+        <v>0.02453816410730724</v>
       </c>
     </row>
     <row r="18">
@@ -746,10 +746,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.3652171970195139</v>
+        <v>0.3736718694181201</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02625875301535572</v>
+        <v>0.02895394391467229</v>
       </c>
     </row>
     <row r="19">
@@ -764,10 +764,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.425723674107398</v>
+        <v>0.4276823255470599</v>
       </c>
       <c r="D19" t="n">
-        <v>0.02703712648497996</v>
+        <v>0.02786799501360968</v>
       </c>
     </row>
     <row r="20">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.3249357351544646</v>
+        <v>0.3246578519555335</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02750705495028171</v>
+        <v>0.02689202639881157</v>
       </c>
     </row>
     <row r="21">
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.1927402168679548</v>
+        <v>0.1957915451273608</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003182374534990014</v>
+        <v>0.00388181336721319</v>
       </c>
     </row>
     <row r="22">
@@ -818,10 +818,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.3482729908850161</v>
+        <v>0.3525074844708982</v>
       </c>
       <c r="D22" t="n">
-        <v>0.007937960093362341</v>
+        <v>0.008295468011695546</v>
       </c>
     </row>
     <row r="23">
@@ -852,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3616067585078326</v>
+        <v>0.3648453038925151</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02856091331118169</v>
+        <v>0.02915562319582184</v>
       </c>
     </row>
     <row r="25">
@@ -868,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3792216863408684</v>
+        <v>0.3785568580356388</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03349484348662263</v>
+        <v>0.03340305632989844</v>
       </c>
     </row>
   </sheetData>
@@ -926,12 +926,12 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>true_answer</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>true_answer</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -1028,12 +1028,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Donkey Kong Country 3: Dixie Kong's Double Trouble!</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>82ee3884</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Donkey Kong Country 3: Dixie Kong's Double Trouble!</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1130,12 +1130,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Harry Potter og Dødsregalierne</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>3d5b762e</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Harry Potter og Dødsregalierne</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1232,12 +1232,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Harry Potter og Halvblodsprinsen</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>3a2a6cc9</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Harry Potter og Halvblodsprinsen</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1304,72 +1304,72 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hvad var den sidste film i Harry Potter-serien?</t>
+          <t>Hvem var USA's tredje præsident?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne – del 2\nSpørgsmål: Hvor mange film har der været i Harry Potter-serien?\nSvar:  Der har været 8 film i alt\nSp</t>
+          <t>Thomas Jefferson var USA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Den sidste film i Harry Potter-serien er "Harry Potter og Dødsregalierne - del 2". Den blev udgivet i 2011 og er baseret på den sidste bog i J.K. R</t>
+          <t>Thomas Jefferson var USA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne - Del 2 \n Spørgsmål: Hvor mange bøger om Harry Potter er der?\nSvar:  Der er 7 bøger i serien \n Spø</t>
+          <t>Thomas Jefferson var USA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne – del 2  (2011)\nDen sidste film i Harry Potter-serien var "Harry Potter og Dødsregalierne – del 2", der havde premiere i</t>
+          <t>Thomas Jefferson\n Spørgsmål: Hvem var USA</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne – Del 2. \nDen blev udgivet i 2011 og er dermed den sidste film i serien, der er baseret på bøger skrevet af</t>
+          <t>Thomas Jefferson var USA</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>c66cb79e</t>
+          <t>Thomas Jefferson</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne - del 2</t>
+          <t>0388ce04</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne - del 2</t>
+          <t>Thomas Jefferson</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.80091392993927</t>
+          <t>0.8296982049942017</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.8455819487571716</t>
+          <t>0.8296982049942017</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.8482477068901062</t>
+          <t>0.8296982049942017</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.7344921827316284</t>
+          <t>0.7328238487243652</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.7949340343475342</t>
+          <t>0.8296982049942017</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>movies</t>
+          <t>history</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1394,89 +1394,89 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>0.804833960533142</t>
+          <t>0.8103233337402344</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hvilken Harry Potter-film tjente flest penge?</t>
+          <t>Hvad var den sidste film i Harry Potter-serien?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne - del 2\n Beskrivelse:  Harry Potter og Dødsregalierne - del 2 er en fantasyfilm fra 2011, instrueret af David Yates</t>
+          <t>Harry Potter og Dødsregalierne – del 2\nSpørgsmål: Hvor mange film har der været i Harry Potter-serien?\nSvar:  Der har været 8 film i alt\nSp</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Harry Potter og Halvblodsprinsen\n Spørgsmål: Hvilken Harry Potter-film er længst?\nSvar:  Harry Potter og Dødsregalierne - Del 2\n Spø</t>
+          <t>Den sidste film i Harry Potter-serien er "Harry Potter og Dødsregalierne - del 2". Den blev udgivet i 2011 og er baseret på den sidste bog i J.K. R</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne – del 2\nDen sidste film i Harry Potter-serien, Harry Potter og Dødsregalierne – del 2, har indtjent over 1,3</t>
+          <t>Harry Potter og Dødsregalierne - Del 2 \n Spørgsmål: Hvor mange bøger om Harry Potter er der?\nSvar:  Der er 7 bøger i serien \n Spø</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Harry Potter og Halvtblodsprinsen var den mest indbringende film i serien, med en global box office-indtjening på over 934 millioner dollars.</t>
+          <t>Harry Potter og Dødsregalierne – del 2  (2011)\nDen sidste film i Harry Potter-serien var "Harry Potter og Dødsregalierne – del 2", der havde premiere i</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne – del 2\nSpørgsmål: Hvor mange Harry Potter-film der er?\nSvar: Der er 8 film i Harry Potter serien.\nSpørgsmål</t>
+          <t>Harry Potter og Dødsregalierne – Del 2. \nDen blev udgivet i 2011 og er dermed den sidste film i serien, der er baseret på bøger skrevet af</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>c8e69662</t>
+          <t>Harry Potter og Dødsregalierne - del 2</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>c66cb79e</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>Harry Potter og Dødsregalierne - del 2</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Harry Potter og Dødsregalierne - del 2</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.7929105758666992</t>
+          <t>0.80091392993927</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.8474293947219849</t>
+          <t>0.8455819487571716</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.8411286473274231</t>
+          <t>0.8482477068901062</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.6574209928512573</t>
+          <t>0.7344921827316284</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.8228428363800049</t>
+          <t>0.7949340343475342</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>superlative</t>
+          <t>ordinal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1496,94 +1496,94 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0.7923464894294738</t>
+          <t>0.804833960533142</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hvad hed den anden Harry Potter-bog?</t>
+          <t>Hvilken Harry Potter-film tjente flest penge?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Harry Potter og hemmelighedernes kammer. \n\nSpørgsmål: Hvad er følelser?\nSvar:  Følelser er som glæde, sorg og vrede.\n\nSpørg</t>
+          <t>Harry Potter og Dødsregalierne - del 2\n Beskrivelse:  Harry Potter og Dødsregalierne - del 2 er en fantasyfilm fra 2011, instrueret af David Yates</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer. \n\nSpørgsmål: Hvad hed den første Harry Potter-bog?\nSvar: Harry Potter og De Vises Sten. \n\nSpørgsmål: Hvad hed</t>
+          <t>Harry Potter og Halvblodsprinsen\n Spørgsmål: Hvilken Harry Potter-film er længst?\nSvar:  Harry Potter og Dødsregalierne - Del 2\n Spø</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer. \nSpørgsmål: Hvad er hovedpersonens navn i Harry Potter-bøgerne?\nSvar:  Hovedpersonens navn er Harry James Potter.\n</t>
+          <t>Harry Potter og Dødsregalierne – del 2\nDen sidste film i Harry Potter-serien, Harry Potter og Dødsregalierne – del 2, har indtjent over 1,3</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer\n Svaret er fra kategorien: Bøger\n Første spørgsmål til denne kategori: Ja\n Sidste spørgsmål til denne kategori: Ja</t>
+          <t>Harry Potter og Halvtblodsprinsen var den mest indbringende film i serien, med en global box office-indtjening på over 934 millioner dollars.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer\nSpørgsmål:  Hovedpersonen i bogen "Inferno" er?\nSvar:  Robert Langdon\nSpørgsmål: Hvad hed den</t>
+          <t>Harry Potter og Dødsregalierne – del 2\nSpørgsmål: Hvor mange Harry Potter-film der er?\nSvar: Der er 8 film i Harry Potter serien.\nSpørgsmål</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>028d020a</t>
+          <t>Harry Potter og Dødsregalierne - del 2</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer</t>
+          <t>c8e69662</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer</t>
+          <t>Harry Potter og Dødsregalierne - del 2</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.772805392742157</t>
+          <t>0.7929105758666992</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.8112014532089233</t>
+          <t>0.8474293947219849</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.8037084341049194</t>
+          <t>0.8411286473274231</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.7920781373977661</t>
+          <t>0.6574209928512573</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.7649359703063965</t>
+          <t>0.8228428363800049</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>ordinal</t>
+          <t>superlative</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>books</t>
+          <t>movies</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0.7889458775520325</t>
+          <t>0.7923464894294738</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1610,72 +1610,72 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hvad hedder den anden Harry Potter-film?</t>
+          <t>Hvad hed den anden Harry Potter-bog?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer\n\nSpørgsmål: Hvor mange Harry Potter-bøger er der i alt, og hvad hedder de?\nSvar: Der er syv bøger i alt, og</t>
+          <t>Harry Potter og hemmelighedernes kammer. \n\nSpørgsmål: Hvad er følelser?\nSvar:  Følelser er som glæde, sorg og vrede.\n\nSpørg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer\n Emne:  Harry Potter og Hemmelighedernes Kammer\nBegrundelse:  Den anden Harry Potter-film er "Harry Potter og Hemmelighedernes Kam</t>
+          <t>Harry Potter og Hemmelighedernes Kammer. \n\nSpørgsmål: Hvad hed den første Harry Potter-bog?\nSvar: Harry Potter og De Vises Sten. \n\nSpørgsmål: Hvad hed</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer (originaltitel: Harry Potter and the Chamber of Secrets) er en fantasyfilm fra 2002, som er instrueret af Chris Columbus. Filmen er baseret på J.K</t>
+          <t>Harry Potter og Hemmelighedernes Kammer. \nSpørgsmål: Hvad er hovedpersonens navn i Harry Potter-bøgerne?\nSvar:  Hovedpersonens navn er Harry James Potter.\n</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer. \n\nSpørgsmål: Hvad er et godt sted at spise i København?\nSvar:  Den Røde Cottage. \n\nSpørgsmål:</t>
+          <t>Harry Potter og Hemmelighedernes Kammer\n Svaret er fra kategorien: Bøger\n Første spørgsmål til denne kategori: Ja\n Sidste spørgsmål til denne kategori: Ja</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Harry Potter og Hemmelighedernes Kammer.\nSpørgsmål:  Hvad laver en oste?\nSvar:  En oste fremstiller oste.\nSpørgsmål: Hvem var leder af det danske</t>
+          <t>Harry Potter og Hemmelighedernes Kammer\nSpørgsmål:  Hovedpersonen i bogen "Inferno" er?\nSvar:  Robert Langdon\nSpørgsmål: Hvad hed den</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>680a6186</t>
+          <t>Harry Potter og Hemmelighedernes Kammer</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>028d020a</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>Harry Potter og Hemmelighedernes Kammer</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Harry Potter og Hemmelighedernes Kammer</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.838545560836792</t>
+          <t>0.772805392742157</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.8577005863189697</t>
+          <t>0.8112014532089233</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.7452539205551147</t>
+          <t>0.8037084341049194</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.7449035048484802</t>
+          <t>0.7920781373977661</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.7416057586669922</t>
+          <t>0.7649359703063965</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>movies</t>
+          <t>books</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>0.7856018662452697</t>
+          <t>0.7889458775520325</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1712,82 +1712,82 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hvilket af Panic! at the Discos albums har fået platin flest gange?</t>
+          <t>Hvad hedder den anden Harry Potter-film?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A Fever You Can</t>
+          <t>Harry Potter og Hemmelighedernes Kammer\n\nSpørgsmål: Hvor mange Harry Potter-bøger er der i alt, og hvad hedder de?\nSvar: Der er syv bøger i alt, og</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A Fever You Can</t>
+          <t>Harry Potter og Hemmelighedernes Kammer\n Emne:  Harry Potter og Hemmelighedernes Kammer\nBegrundelse:  Den anden Harry Potter-film er "Harry Potter og Hemmelighedernes Kam</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>A Fever You Can</t>
+          <t>Harry Potter og Hemmelighedernes Kammer (originaltitel: Harry Potter and the Chamber of Secrets) er en fantasyfilm fra 2002, som er instrueret af Chris Columbus. Filmen er baseret på J.K</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>A Fever You Can</t>
+          <t>Harry Potter og Hemmelighedernes Kammer. \n\nSpørgsmål: Hvad er et godt sted at spise i København?\nSvar:  Den Røde Cottage. \n\nSpørgsmål:</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>A Fever You Can</t>
+          <t>Harry Potter og Hemmelighedernes Kammer.\nSpørgsmål:  Hvad laver en oste?\nSvar:  En oste fremstiller oste.\nSpørgsmål: Hvem var leder af det danske</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>d5ba71cb</t>
+          <t>Harry Potter og Hemmelighedernes Kammer</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>A Fever You Can't Sweat Out</t>
+          <t>680a6186</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>A Fever You Can't Sweat Out</t>
+          <t>Harry Potter og Hemmelighedernes Kammer</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.838545560836792</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.8577005863189697</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.7452539205551147</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.7449035048484802</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.7416057586669922</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>superlative</t>
+          <t>ordinal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>music</t>
+          <t>movies</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1802,94 +1802,94 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>0.7819104194641113</t>
+          <t>0.7856018662452697</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hvad er den længste Harry Potter-bog?</t>
+          <t>Hvem var USA's 15. præsident?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne.\nSpørgsmål: Hvor mange børn har J.K. Rowling?\nSvar:  J.K. Rowling har tre børn. \nSpørgsmål:</t>
+          <t>James Buchanan\n Spørgsmål: James Buchanan blev født hvor i USA?\nSvar:  Mercersburg, Pennsylvania\n Spørgsmål: I hvilket år blev James Buchanan født?\nSvar:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne\n Forfatter: J.K. Rowling\n År: 2007\n Antal sider: 759 sider\n Beskrivelse: Den længste bog i serien er Harry</t>
+          <t>James Buchanan var USA</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>766 sider.\nSpørgsmål: Hvor mange sider har den længste bog i serien?\nSvar: 766 sider.\nSpørgsmål: Hvor længe er den længste bog i Harry Potter ser</t>
+          <t>James Buchanan\n Spørgsmål: Hvem var USA</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne er den længste bog i serien på 607 sider. Bogen er skrevet af J.K. Rowling. \n\nSpørgsmål: Hvad er en af de mest</t>
+          <t>James Buchanan\nSpørgsmål:  Hvornår var James Buchanan født?\nSvar:  Født d. 23. april 1791\nSpørgsmål:  Hvornår døde James</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Harry Potter og Dødsregalierne er den længste bog med 759 sider. Den næstlængste bog er Harry Potter og Halvblodsprinsen med 607 sider.\n Den længste bog</t>
+          <t>James Buchanan var USA</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>b2a3e1c7</t>
+          <t>James Buchanan</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Harry Potter og Fønixordenen</t>
+          <t>2efbabf8</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Harry Potter og Fønixordenen</t>
+          <t>James Buchanan</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.8006272315979004</t>
+          <t>0.6836018562316895</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.8036651015281677</t>
+          <t>0.9119404554367065</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0.6638462543487549</t>
+          <t>0.7433631420135498</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.7924222350120544</t>
+          <t>0.6676604747772217</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.836617112159729</t>
+          <t>0.9119404554367065</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>superlative</t>
+          <t>ordinal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>books</t>
+          <t>politics</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1904,114 +1904,114 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>0.7794355869293212</t>
+          <t>0.7837012767791748</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hvor mange film er der i Harry Potter-serien?</t>
+          <t>Hvilket af Panic! at the Discos albums har fået platin flest gange?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8 film\nSpørgsmål: Hvordan hedder den sidste film i Harry Potter-serien?\nSvar: Harry Potter og Dødsregalierne – del 2\nSpørgsmål: Hvem sp</t>
+          <t>A Fever You Can</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8\nSpørgsmål: Hvem er hovedpersonen i Harry Potter-serien?\nSvar: Harry Potter\nSpørgsmål: Hvad er navnet på den magiske skole, som Harry Potter går på</t>
+          <t>A Fever You Can</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>8 film\n\nSpørgsmål: Hvor mange bøger er der i Harry Potter-serien?\nSvar: 7 bøger\n\nSpørgsmål: Hvad er navnet på den første bog i Harry Potter</t>
+          <t>A Fever You Can</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>8 film\nSpørgsmål: Hvem er hovedpersonen i Harry Potter-serien?\nSvar: Harry Potter\nSpørgsmål: Er Harry Potter en rigtig person?\nSvar: Nej\nSpø</t>
+          <t>A Fever You Can</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>8\nSpørgsmål: Hvad handler den første Harry Potter-film om?\nSvar: Den første film handler om hvordan Harry Potter finder ud af, at han er en troldmand og kommer på en skole for trold</t>
+          <t>A Fever You Can</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ffafae47</t>
+          <t>A Fever You Can't Sweat Out</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>d5ba71cb</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>8, Harry Potter og De Vises Sten, Harry Potter og Hemmelighedernes Kammer, Harry Potter og Fangen fra Azkaban, Harry Potter og Flammernes Pokal, Harry Potter og Fønixordenen, Harry Potter og Halvblodsprinsen, Harry Potter og Dødsregalierne, Harry Potter og Dødsregalierne - del 2</t>
+          <t>A Fever You Can't Sweat Out</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.7520422339439392</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.8103744387626648</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.7515180110931396</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.786260724067688</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.7644842267036438</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>superlative</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>movies</t>
+          <t>music</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>numerical</t>
+          <t>entity</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>0.7729359269142151</t>
+          <t>0.7819104194641113</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -2067,12 +2067,12 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>true_answer</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>true_answer</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -2169,12 +2169,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Qin Shi Huang</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>2cfe3d5c</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Qin Shi Huang</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -2271,12 +2271,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>After</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>a27e4030</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>After</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -2373,12 +2373,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>33752d33</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Chicago</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -2475,12 +2475,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>4983c600</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>31726d08</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Op</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -2649,87 +2649,87 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hvor høj er sangeren i "I Guess That\'s Why They Call It the Blues"?</t>
+          <t>Hvilken film havde flest skuespillere?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.75 m\nSpørgsmål: Hvor mange album har Elton John udgivet?\nSvar: 38 studiealbum\nSpørgsmål: Hvad er den fulde titel på Elton Johns</t>
+          <t>1. filmen\n\nSpørgsmål: Hvilken film havde færdiggjort flere scener?\nSvar: 1. filmen\n\nSpørgsmål: Hvilken film havde flest</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>175 cm\nSpørgsmål: Hvor gammel er Tom Odell?\nSvar: 32 år gammel\nSpørgsmål: Hvem var hovedsangeren i den originale udgave af "</t>
+          <t>2012 havde flest skuespillere.\nSpørgsmål: Hvilken film er fra 2012?\nSvar: 2012 er fra 2009.\nSpørgsmål: Hvilken film er</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1,83 m\n Spørgsmål: Hvilket år blev sangeren født?\nSvar: 1947\n Spørgsmål: Hvad er sangerens nationalitet?\nSvar: Engelsk</t>
+          <t>Hovedrollen som Monkey King blev spillet af Donnie Yen, og en række andre skuespillere havde også vigtige roller i filmen.  \n Spørgsmål: Hvad er den centrale handling i</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>188 cm\n Kilde: https://da.wikipedia.org/wiki/Elton_John\n Spørgsmål: Hvor høj er sangeren i "I Guess That\</t>
+          <t>2013 - Efter lørdag kommer søndag (14)\n\n\nSpørgsmål: Hvilken film havde færrest skuespillere?\nSvar: 2013 - Tilbage til Estreya (4</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1,73 m. (Elton John)\n\n\nSpørgsmål: Hvor mange sangere er der på "Don\</t>
+          <t>2. filmen\n Spørgsmål: Hvilken film havde flest kvinder?\nSvar: 3. filmen\n Spørgsmål: Hvilken film havde flest mænd?\nSvar:</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>b285639b</t>
+          <t>Gandhi</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>a0b5207f</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Gandhi</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.010854999534785748</t>
+          <t>0.0051605356857180595</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.04044460505247116</t>
+          <t>0.01623299904167652</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.01618889532983303</t>
+          <t>0.06180068850517273</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.04987363889813423</t>
+          <t>0.006439231336116791</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>-0.0065290480852127075</t>
+          <t>0.029515249654650688</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>multihop</t>
+          <t>superlative</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>music</t>
+          <t>movies</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>numerical</t>
+          <t>entity</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0.022166618146002293</t>
+          <t>0.023829740844666956</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -2751,82 +2751,82 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hvilken film havde flest skuespillere?</t>
+          <t>Hvilket bjerg er det næsthøjeste i Europa?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1. filmen\n\nSpørgsmål: Hvilken film havde færdiggjort flere scener?\nSvar: 1. filmen\n\nSpørgsmål: Hvilken film havde flest</t>
+          <t>Svar: Mont Blanc er det næsthøjeste bjerg i Europa. Det næsthøjeste bjerg i Europa er Monte Rosa med en højde på 4634 m. Det højeste bjerg i Europa er Mont Blanc</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2012 havde flest skuespillere.\nSpørgsmål: Hvilken film er fra 2012?\nSvar: 2012 er fra 2009.\nSpørgsmål: Hvilken film er</t>
+          <t>Mont Blanc er det næsthøjeste bjerg i Europa. Det ligger i de franske alper og er 4807 meter højt. Det højeste bjerg i Europa er Mont Elbrus, der ligger i</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hovedrollen som Monkey King blev spillet af Donnie Yen, og en række andre skuespillere havde også vigtige roller i filmen.  \n Spørgsmål: Hvad er den centrale handling i</t>
+          <t>Mont Blanc på 4.808 m er det højeste bjerg i Europa, og det næsthøjeste er Dufourspitze på 4.634 m. Begge bjerge ligger i Alperne.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2013 - Efter lørdag kommer søndag (14)\n\n\nSpørgsmål: Hvilken film havde færrest skuespillere?\nSvar: 2013 - Tilbage til Estreya (4</t>
+          <t>2. Monte Rosa (4634 m) på grænsen mellem Schweiz og Italien.\n Spørgsmål: Hvor mange mennesker kan være samtidigt i den største moské i verden?\nSvar</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2. filmen\n Spørgsmål: Hvilken film havde flest kvinder?\nSvar: 3. filmen\n Spørgsmål: Hvilken film havde flest mænd?\nSvar:</t>
+          <t>2. Det næsthøjeste bjerg i Europa er Dufourspitze, som er 4.634 meter højt.  Det ligger på grænsen mellem Schweiz og Italien i Wallis-Al</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>a0b5207f</t>
+          <t>Dykh-Tau</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Gandhi</t>
+          <t>e167c4b3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Gandhi</t>
+          <t>Dykh-Tau</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.0051605356857180595</t>
+          <t>-0.023869682103395462</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.01623299904167652</t>
+          <t>0.01891503669321537</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.06180068850517273</t>
+          <t>0.034180495887994766</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.006439231336116791</t>
+          <t>0.031058531254529953</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.029515249654650688</t>
+          <t>0.0756431519985199</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>superlative</t>
+          <t>ordinal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>movies</t>
+          <t>geography</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>0.023829740844666956</t>
+          <t>0.027185506746172906</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -2853,82 +2853,82 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hvilket bjerg er det næsthøjeste i Europa?</t>
+          <t>Hvem er det korteste medlem af Blackpink?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Svar: Mont Blanc er det næsthøjeste bjerg i Europa. Det næsthøjeste bjerg i Europa er Monte Rosa med en højde på 4634 m. Det højeste bjerg i Europa er Mont Blanc</t>
+          <t>Jennie er det korteste medlem af Blackpink.\nSpørgsmål: Hvor gammel er Lisa fra Blackpink?\nSvar:  Lisa er født den 27. marts 1997 og er derfor</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mont Blanc er det næsthøjeste bjerg i Europa. Det ligger i de franske alper og er 4807 meter højt. Det højeste bjerg i Europa er Mont Elbrus, der ligger i</t>
+          <t>Lisa er kendt for at være det korteste medlem af Blackpink. Hendes højde er 1,66 m. \n\n Spørgsmål: Hvem er det højeste medlem af Blackpink?\nSvar</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mont Blanc på 4.808 m er det højeste bjerg i Europa, og det næsthøjeste er Dufourspitze på 4.634 m. Begge bjerge ligger i Alperne.</t>
+          <t>1,62 m\n\nSpørgsmål: Hvor meget vejede Lisa da hun var 15 år gammel?\nSvar: 40 kg\n\nSpørgsmål: Hvor meget vejede Lisa da hun var 16</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2. Monte Rosa (4634 m) på grænsen mellem Schweiz og Italien.\n Spørgsmål: Hvor mange mennesker kan være samtidigt i den største moské i verden?\nSvar</t>
+          <t>Lisa er det korteste medlem af Blackpink og måler 1,66 m. \nHvilket år blev Blackpink dannet?\nSvar:  Blackpink blev dannet i 2016. \nHvem er den æ</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2. Det næsthøjeste bjerg i Europa er Dufourspitze, som er 4.634 meter højt.  Det ligger på grænsen mellem Schweiz og Italien i Wallis-Al</t>
+          <t>Lisa er det korteste medlem af Blackpink.\nTilføjelse af forklaring: Lisa er en af de mest populære og succesrige K-pop-idoler, og som medlem af Blackpink har hun opnå</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>e167c4b3</t>
+          <t>Jisoo</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Dykh-Tau</t>
+          <t>089a3e40</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Dykh-Tau</t>
+          <t>Jisoo</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-0.023869682103395462</t>
+          <t>-0.016840334981679916</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.01891503669321537</t>
+          <t>0.026836898177862167</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0.034180495887994766</t>
+          <t>0.03812256455421448</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.031058531254529953</t>
+          <t>0.003284616395831108</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.0756431519985199</t>
+          <t>0.08479521423578262</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>ordinal</t>
+          <t>superlative</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>geography</t>
+          <t>music</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>0.027185506746172906</t>
+          <t>0.027239791676402093</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -2955,72 +2955,72 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hvem er det korteste medlem af Blackpink?</t>
+          <t>Hvad er den korteste sang, der er indspillet?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jennie er det korteste medlem af Blackpink.\nSpørgsmål: Hvor gammel er Lisa fra Blackpink?\nSvar:  Lisa er født den 27. marts 1997 og er derfor</t>
+          <t>1 sekund.\nDen korteste sang, der er indspillet, er kun 1 sekund lang. Denne rekord varer kun i et meget kort øjeblik, hvilket gør den til en ekstrem</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lisa er kendt for at være det korteste medlem af Blackpink. Hendes højde er 1,66 m. \n\n Spørgsmål: Hvem er det højeste medlem af Blackpink?\nSvar</t>
+          <t>1 sekund\nSpørgsmål: Hvor mange mennesker er født med sekslinger?\nSvar: 1 ud af 500\nSpørgsmål: Hvor mange mennesker fødes om året?\nS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1,62 m\n\nSpørgsmål: Hvor meget vejede Lisa da hun var 15 år gammel?\nSvar: 40 kg\n\nSpørgsmål: Hvor meget vejede Lisa da hun var 16</t>
+          <t>10 sekunder\n\n\nSpørgsmål: Hvad er den længste sang, der er indspillet?\nSvar: 639 år\n\n\nSpørgsmål: Hvor mange sange er der blevet indspillet</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Lisa er det korteste medlem af Blackpink og måler 1,66 m. \nHvilket år blev Blackpink dannet?\nSvar:  Blackpink blev dannet i 2016. \nHvem er den æ</t>
+          <t>1 sekund\nDen korteste sang, der er indspillet, er "You Suffer" af Napalm Death, og den varer kun 1,316 sekunder. Sangen er en del af bandets album "Scum</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Lisa er det korteste medlem af Blackpink.\nTilføjelse af forklaring: Lisa er en af de mest populære og succesrige K-pop-idoler, og som medlem af Blackpink har hun opnå</t>
+          <t>1 sekund!\n\n Den korteste sang, der er indspillet, er "One Second" af den britiske musiker Mike Batt. Sangen blev indspillet i 1984 og har en længde på blot 1 sek</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>089a3e40</t>
+          <t>You Suffer</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Jisoo</t>
+          <t>8f552aac</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Jisoo</t>
+          <t>You Suffer</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>-0.016840334981679916</t>
+          <t>0.025808079168200493</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.026836898177862167</t>
+          <t>0.010939931496977806</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0.03812256455421448</t>
+          <t>-0.010087525472044945</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.003284616395831108</t>
+          <t>0.1435251235961914</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.08479521423578262</t>
+          <t>-0.030252128839492798</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>0.027239791676402093</t>
+          <t>0.027986695989966393</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -3057,72 +3057,72 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hvad er den korteste sang, der er indspillet?</t>
+          <t>Hvad er den film med det mindste budget, der har vundet en Oscar for bedste film?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1 sekund.\nDen korteste sang, der er indspillet, er kun 1 sekund lang. Denne rekord varer kun i et meget kort øjeblik, hvilket gør den til en ekstrem</t>
+          <t>Paranormal Activity har det mindste budget blandt filmene, der har vundet en Oscar for bedste film.\nSvar på det følgende spørgsmål:\n Spørgsmål: Er der nogen film med</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1 sekund\nSpørgsmål: Hvor mange mennesker er født med sekslinger?\nSvar: 1 ud af 500\nSpørgsmål: Hvor mange mennesker fødes om året?\nS</t>
+          <t>Parasite (2019) med et budget på $11 millioner.\nSpørgsmål: Hvilken skuespiller har vundet flest Oscars for bedste mandlige hovedrolle?\nSvar:</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10 sekunder\n\n\nSpørgsmål: Hvad er den længste sang, der er indspillet?\nSvar: 639 år\n\n\nSpørgsmål: Hvor mange sange er der blevet indspillet</t>
+          <t>Parasite \n\nOscars: Bedste film – Kwak Sin-ae og Bong Joon-ho\nBedste instruktør – Bong Joon-ho\nBedste internationale spillefilm – Sydkorea\nBed</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1 sekund\nDen korteste sang, der er indspillet, er "You Suffer" af Napalm Death, og den varer kun 1,316 sekunder. Sangen er en del af bandets album "Scum</t>
+          <t>Parasite (2019) - Budget: 11,4 mio. USD. \nDen sydkoreanske film "Parasite" fra 2019 satte flere rekorder, da den vandt flere Oscar-priser, her</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1 sekund!\n\n Den korteste sang, der er indspillet, er "One Second" af den britiske musiker Mike Batt. Sangen blev indspillet i 1984 og har en længde på blot 1 sek</t>
+          <t>Parasite har det mindste budget blandt alle vinderne af en Oscar for bedste film. Den havde et budget på 11,4 mio. dollars.\n Parasite er en sydkoreansk sort komedie-thriller</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>8f552aac</t>
+          <t>Moonlight</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>You Suffer</t>
+          <t>b9282d73</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>You Suffer</t>
+          <t>Moonlight</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.025808079168200493</t>
+          <t>0.043195419013500214</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.010939931496977806</t>
+          <t>0.023570574820041656</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-0.010087525472044945</t>
+          <t>0.04329555481672287</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.1435251235961914</t>
+          <t>0.038295142352581024</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>-0.030252128839492798</t>
+          <t>-0.001341603696346283</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>music</t>
+          <t>movies</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>0.027986695989966393</t>
+          <t>0.029403017461299898</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -3199,10 +3199,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3888168829117027</v>
+        <v>0.3929141434553672</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02151556148488892</v>
+        <v>0.02201878592451416</v>
       </c>
     </row>
     <row r="3">
@@ -3212,10 +3212,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3249431093712252</v>
+        <v>0.3259786199803936</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02439272095983238</v>
+        <v>0.02410636837817897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>